<commit_message>
Added TC001 , TC002 and TC003 for Test Plan Tab
</commit_message>
<xml_diff>
--- a/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
+++ b/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
@@ -1,37 +1,36 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
-  <workbookPr/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0794A050-4157-4D03-B39B-9962F7A763A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SohailShaikhFaiyaz\Desktop\UAT\testData\testPlanTabTestData\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
+    <sheet name="tc002" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="191028"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
-      <x15:workbookPr chartTrackingRefBase="1"/>
-    </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
-  </extLst>
+  <calcPr/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <si>
+    <t>projectName</t>
+  </si>
+  <si>
+    <t>SET- DRV</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <fonts count="1">
     <font>
       <sz val="11"/>
@@ -50,13 +49,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
+    <border/>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -69,14 +62,6 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
 </styleSheet>
 </file>
 
@@ -85,10 +70,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -257,6 +242,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -283,24 +269,25 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="12700" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="19050" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln w="25400" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -361,50 +348,48 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
-  <a:objectDefaults>
-    <a:lnDef>
-      <a:spPr/>
-      <a:bodyPr/>
-      <a:lstStyle/>
-      <a:style>
-        <a:lnRef idx="2">
-          <a:schemeClr val="accent1"/>
-        </a:lnRef>
-        <a:fillRef idx="0">
-          <a:schemeClr val="accent1"/>
-        </a:fillRef>
-        <a:effectRef idx="1">
-          <a:schemeClr val="accent1"/>
-        </a:effectRef>
-        <a:fontRef idx="minor">
-          <a:schemeClr val="tx1"/>
-        </a:fontRef>
-      </a:style>
-    </a:lnDef>
-  </a:objectDefaults>
-  <a:extraClrSchemeLst/>
-  <a:extLst>
-    <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
-    </a:ext>
-  </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1"/>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added TC004 and TC005
</commit_message>
<xml_diff>
--- a/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
+++ b/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
@@ -8,11 +8,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
     <sheet name="tc002" sheetId="2" r:id="rId2"/>
+    <sheet name="tc004" sheetId="3" r:id="rId3"/>
+    <sheet name="tc005" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr/>
 </workbook>
@@ -25,6 +27,24 @@
   </si>
   <si>
     <t>SET- DRV</t>
+  </si>
+  <si>
+    <t>ReleaseName</t>
+  </si>
+  <si>
+    <t>SecondReleaseName</t>
+  </si>
+  <si>
+    <t>Release 039</t>
+  </si>
+  <si>
+    <t>releaseName</t>
+  </si>
+  <si>
+    <t>STG- PulseCodeOnAzureCloud</t>
+  </si>
+  <si>
+    <t>Test_Sohail</t>
   </si>
 </sst>
 </file>
@@ -371,7 +391,7 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
@@ -392,4 +412,70 @@
     </row>
   </sheetData>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
+    <col min="2" max="2" width="20.25" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.25"/>
+  <cols>
+    <col min="1" max="1" width="27.25" customWidth="1"/>
+    <col min="2" max="2" width="20.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
tc006,tc007 added for test plan
</commit_message>
<xml_diff>
--- a/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
+++ b/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
@@ -1,27 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="29318"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SohailShaikhFaiyaz\Desktop\UAT\testData\testPlanTabTestData\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:dbsheet="http://web.wps.cn/et/2021/dbsheet">
+  <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="3"/>
+    <workbookView windowWidth="19200" windowHeight="6080" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
     <sheet name="tc002" sheetId="2" r:id="rId2"/>
     <sheet name="tc004" sheetId="3" r:id="rId3"/>
     <sheet name="tc005" sheetId="4" r:id="rId4"/>
+    <sheet name="tc006" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
   <si>
     <t>projectName</t>
   </si>
@@ -45,43 +55,707 @@
   </si>
   <si>
     <t>Test_Sohail</t>
+  </si>
+  <si>
+    <t>Project Name</t>
+  </si>
+  <si>
+    <t>release name</t>
+  </si>
+  <si>
+    <t>testCycle name</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Mayukh_Release</t>
+  </si>
+  <si>
+    <t>Mayukh_TestCycle</t>
+  </si>
+  <si>
+    <t>Hi,this is the description</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
+  <numFmts count="4">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+  </numFmts>
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
-      <family val="2"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
-    <border/>
+  <borders count="9">
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
+    <cellStyle name="Currency" xfId="2" builtinId="4"/>
+    <cellStyle name="Percent" xfId="3" builtinId="5"/>
+    <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
+    <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
+    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
+    <cellStyle name="Note" xfId="8" builtinId="10"/>
+    <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
+    <cellStyle name="Title" xfId="10" builtinId="15"/>
+    <cellStyle name="CExplanatory Text" xfId="11" builtinId="53"/>
+    <cellStyle name="Heading 1" xfId="12" builtinId="16"/>
+    <cellStyle name="Heading 2" xfId="13" builtinId="17"/>
+    <cellStyle name="Heading 3" xfId="14" builtinId="18"/>
+    <cellStyle name="Heading 4" xfId="15" builtinId="19"/>
+    <cellStyle name="Input" xfId="16" builtinId="20"/>
+    <cellStyle name="Output" xfId="17" builtinId="21"/>
+    <cellStyle name="Calculation" xfId="18" builtinId="22"/>
+    <cellStyle name="Check Cell" xfId="19" builtinId="23"/>
+    <cellStyle name="Linked Cell" xfId="20" builtinId="24"/>
+    <cellStyle name="Total" xfId="21" builtinId="25"/>
+    <cellStyle name="Good" xfId="22" builtinId="26"/>
+    <cellStyle name="Bad" xfId="23" builtinId="27"/>
+    <cellStyle name="Neutral" xfId="24" builtinId="28"/>
+    <cellStyle name="Accent1" xfId="25" builtinId="29"/>
+    <cellStyle name="20% - Accent1" xfId="26" builtinId="30"/>
+    <cellStyle name="40% - Accent1" xfId="27" builtinId="31"/>
+    <cellStyle name="60% - Accent1" xfId="28" builtinId="32"/>
+    <cellStyle name="Accent2" xfId="29" builtinId="33"/>
+    <cellStyle name="20% - Accent2" xfId="30" builtinId="34"/>
+    <cellStyle name="40% - Accent2" xfId="31" builtinId="35"/>
+    <cellStyle name="60% - Accent2" xfId="32" builtinId="36"/>
+    <cellStyle name="Accent3" xfId="33" builtinId="37"/>
+    <cellStyle name="20% - Accent3" xfId="34" builtinId="38"/>
+    <cellStyle name="40% - Accent3" xfId="35" builtinId="39"/>
+    <cellStyle name="60% - Accent3" xfId="36" builtinId="40"/>
+    <cellStyle name="Accent4" xfId="37" builtinId="41"/>
+    <cellStyle name="20% - Accent4" xfId="38" builtinId="42"/>
+    <cellStyle name="40% - Accent4" xfId="39" builtinId="43"/>
+    <cellStyle name="60% - Accent4" xfId="40" builtinId="44"/>
+    <cellStyle name="Accent5" xfId="41" builtinId="45"/>
+    <cellStyle name="20% - Accent5" xfId="42" builtinId="46"/>
+    <cellStyle name="40% - Accent5" xfId="43" builtinId="47"/>
+    <cellStyle name="60% - Accent5" xfId="44" builtinId="48"/>
+    <cellStyle name="Accent6" xfId="45" builtinId="49"/>
+    <cellStyle name="20% - Accent6" xfId="46" builtinId="50"/>
+    <cellStyle name="40% - Accent6" xfId="47" builtinId="51"/>
+    <cellStyle name="60% - Accent6" xfId="48" builtinId="52"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -90,10 +764,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -128,7 +802,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="020F0302020204030204"/>
+        <a:latin typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -161,26 +835,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -213,23 +870,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -373,61 +1013,72 @@
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14"/>
   <sheetData/>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="23.625" customWidth="1"/>
+    <col min="1" max="1" width="23.6272727272727" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:1">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:1">
       <c r="A2" t="s">
         <v>1</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection activeCell="B3" sqref="A1:B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="21.375" customWidth="1"/>
-    <col min="2" max="2" width="20.25" customWidth="1"/>
+    <col min="1" max="1" width="21.3727272727273" customWidth="1"/>
+    <col min="2" max="2" width="20.2545454545455" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
         <v>2</v>
       </c>
@@ -435,7 +1086,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:2">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -444,38 +1095,95 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
+  <cols>
+    <col min="1" max="1" width="27.2545454545455" customWidth="1"/>
+    <col min="2" max="2" width="20.7545454545455" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="1" width="27.25" customWidth="1"/>
-    <col min="2" max="2" width="20.75" customWidth="1"/>
+    <col min="1" max="1" width="29" customWidth="1"/>
+    <col min="2" max="2" width="17.4545454545455" customWidth="1"/>
+    <col min="3" max="3" width="30.5454545454545" customWidth="1"/>
+    <col min="4" max="4" width="33.9090909090909" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1">
+    <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>8</v>
       </c>
       <c r="B1" t="s">
-        <v>5</v>
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
       </c>
     </row>
-    <row r="2">
+    <row r="2" spans="1:4">
       <c r="A2" t="s">
         <v>6</v>
       </c>
       <c r="B2" t="s">
-        <v>7</v>
+        <v>12</v>
+      </c>
+      <c r="C2" t="s">
+        <v>13</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
TC011 and TC012 pushed
</commit_message>
<xml_diff>
--- a/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
+++ b/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6080" activeTab="4"/>
+    <workbookView windowWidth="19200" windowHeight="6800" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="tc001" sheetId="1" r:id="rId1"/>
@@ -12,6 +12,7 @@
     <sheet name="tc004" sheetId="3" r:id="rId3"/>
     <sheet name="tc005" sheetId="4" r:id="rId4"/>
     <sheet name="tc006" sheetId="5" r:id="rId5"/>
+    <sheet name="tc011" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -31,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="21">
   <si>
     <t>projectName</t>
   </si>
@@ -76,6 +77,24 @@
   </si>
   <si>
     <t>Hi,this is the description</t>
+  </si>
+  <si>
+    <t>release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">testCycle </t>
+  </si>
+  <si>
+    <t>testSuit</t>
+  </si>
+  <si>
+    <t>Release J10</t>
+  </si>
+  <si>
+    <t>TestCycle 10</t>
+  </si>
+  <si>
+    <t>TestSuite 10</t>
   </si>
 </sst>
 </file>
@@ -83,19 +102,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="xr9">
   <numFmts count="4">
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
-    <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="177" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="178" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="179" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
   </numFmts>
-  <fonts count="21">
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Aptos Narrow"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -551,148 +563,148 @@
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="3" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -706,7 +718,7 @@
     <cellStyle name="Percent" xfId="3" builtinId="5"/>
     <cellStyle name="Comma [0]" xfId="4" builtinId="6"/>
     <cellStyle name="Currency [0]" xfId="5" builtinId="7"/>
-    <cellStyle name="Hyperlink" xfId="6" builtinId="8"/>
+    <cellStyle name="Link" xfId="6" builtinId="8"/>
     <cellStyle name="Followed Hyperlink" xfId="7" builtinId="9"/>
     <cellStyle name="Note" xfId="8" builtinId="10"/>
     <cellStyle name="Warning Text" xfId="9" builtinId="11"/>
@@ -1044,7 +1056,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1"/>
   <cols>
-    <col min="1" max="1" width="23.6272727272727" customWidth="1"/>
+    <col min="1" max="1" width="23.625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:1">
@@ -1074,8 +1086,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="21.3727272727273" customWidth="1"/>
-    <col min="2" max="2" width="20.2545454545455" customWidth="1"/>
+    <col min="1" max="1" width="21.375" customWidth="1"/>
+    <col min="2" max="2" width="20.2583333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1111,8 +1123,8 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="27.2545454545455" customWidth="1"/>
-    <col min="2" max="2" width="20.7545454545455" customWidth="1"/>
+    <col min="1" max="1" width="27.2583333333333" customWidth="1"/>
+    <col min="2" max="2" width="20.7583333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -1142,16 +1154,16 @@
   <sheetPr/>
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="8.725" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="17.4545454545455" customWidth="1"/>
-    <col min="3" max="3" width="30.5454545454545" customWidth="1"/>
-    <col min="4" max="4" width="33.9090909090909" customWidth="1"/>
+    <col min="2" max="2" width="17.4583333333333" customWidth="1"/>
+    <col min="3" max="3" width="30.5416666666667" customWidth="1"/>
+    <col min="4" max="4" width="33.9083333333333" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4">
@@ -1180,6 +1192,57 @@
       </c>
       <c r="D2" t="s">
         <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:D2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="3"/>
+  <cols>
+    <col min="1" max="1" width="32.4166666666667" customWidth="1"/>
+    <col min="2" max="2" width="22.5" customWidth="1"/>
+    <col min="3" max="3" width="20.4166666666667" customWidth="1"/>
+    <col min="4" max="4" width="14.3333333333333" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4">
+      <c r="A1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B1" t="s">
+        <v>15</v>
+      </c>
+      <c r="C1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C2" t="s">
+        <v>19</v>
+      </c>
+      <c r="D2" t="s">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ran the suite and report generated
</commit_message>
<xml_diff>
--- a/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
+++ b/testData/testPlanTabTestData/testPlanTab_TestData.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="19200" windowHeight="6800"/>
+    <workbookView windowWidth="19200" windowHeight="6800" firstSheet="4" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="tc002" sheetId="2" r:id="rId1"/>
@@ -21,6 +21,7 @@
     <sheet name="tc015" sheetId="11" r:id="rId12"/>
     <sheet name="tc018" sheetId="15" r:id="rId13"/>
     <sheet name="tc019" sheetId="14" r:id="rId14"/>
+    <sheet name="tc003" sheetId="16" r:id="rId15"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="82" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="39">
   <si>
     <t>projectName</t>
   </si>
@@ -1157,8 +1158,8 @@
   <sheetPr/>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A1:A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1399,13 +1400,40 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D11" sqref="D11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="8.72727272727273" defaultRowHeight="14" outlineLevelRow="1"/>
+  <sheetData>
+    <row r="1" spans="1:1">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="2" outlineLevelCol="1"/>
@@ -1442,7 +1470,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:B2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>
@@ -1475,7 +1503,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14" outlineLevelRow="1" outlineLevelCol="1"/>

</xml_diff>